<commit_message>
Inclusão e novos arquivos
</commit_message>
<xml_diff>
--- a/downloads/auto-filtro-como-usar-filtrar.xlsx
+++ b/downloads/auto-filtro-como-usar-filtrar.xlsx
@@ -636,7 +636,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -658,12 +658,23 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF0000FF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -679,24 +690,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>63401</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="5" name="Agrupar 4">
-          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" tooltip="Clique aqui para acessar"/>
+        <xdr:cNvPr id="11" name="Agrupar 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C884EBC5-84C1-41DF-8952-08D0C027A93D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A751D8EE-2707-486A-880B-3058917D604E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -704,90 +714,740 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="7381875" y="361950"/>
-          <a:ext cx="3629025" cy="3311426"/>
-          <a:chOff x="5419724" y="628650"/>
-          <a:chExt cx="3629025" cy="3311426"/>
+          <a:off x="6791325" y="409575"/>
+          <a:ext cx="5514975" cy="3409950"/>
+          <a:chOff x="6743700" y="352425"/>
+          <a:chExt cx="5514975" cy="3409950"/>
         </a:xfrm>
       </xdr:grpSpPr>
-      <xdr:pic>
-        <xdr:nvPicPr>
-          <xdr:cNvPr id="6" name="Imagem 5">
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="3" name="CaixaDeTexto 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6356E056-A39E-4075-9D85-76AE757193F9}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B26BD838-3471-4F8F-AC4B-A867519A5029}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
-          <xdr:cNvPicPr>
-            <a:picLocks noChangeAspect="1"/>
-          </xdr:cNvPicPr>
-        </xdr:nvPicPr>
-        <xdr:blipFill>
-          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
-            <a:extLst>
-              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-              </a:ext>
-            </a:extLst>
-          </a:blip>
-          <a:stretch>
-            <a:fillRect/>
-          </a:stretch>
-        </xdr:blipFill>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="5419724" y="1104900"/>
-            <a:ext cx="3629025" cy="2835176"/>
+            <a:off x="6743700" y="352425"/>
+            <a:ext cx="5514975" cy="3409950"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
             <a:avLst/>
           </a:prstGeom>
-        </xdr:spPr>
-      </xdr:pic>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="7" name="Retângulo 6">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{31B26791-CF8C-43B3-BD80-0CFDABA767F6}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="5429250" y="628650"/>
-            <a:ext cx="3600450" cy="466725"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:ln w="3175"/>
+          <a:solidFill>
+            <a:schemeClr val="lt1"/>
+          </a:solidFill>
+          <a:ln w="9525" cmpd="sng">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="65000"/>
+                <a:lumOff val="35000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
         </xdr:spPr>
         <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent3"/>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
           </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="lt1"/>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
           </a:fillRef>
           <a:effectRef idx="0">
-            <a:schemeClr val="accent3"/>
+            <a:scrgbClr r="0" g="0" b="0"/>
           </a:effectRef>
           <a:fontRef idx="minor">
             <a:schemeClr val="dk1"/>
           </a:fontRef>
         </xdr:style>
         <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
           <a:lstStyle/>
           <a:p>
-            <a:pPr algn="ctr"/>
+            <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr/>
+            </a:pPr>
             <a:r>
-              <a:rPr lang="pt-BR" sz="1400" b="1"/>
-              <a:t>DICA DE 1 MILHÃO DE DÓLARES</a:t>
+              <a:rPr lang="pt-BR" sz="2000" b="1" i="0">
+                <a:solidFill>
+                  <a:srgbClr val="0070C0"/>
+                </a:solidFill>
+                <a:effectLst/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:rPr>
+              <a:t>DICA</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="2000" b="1" i="0" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="0070C0"/>
+                </a:solidFill>
+                <a:effectLst/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:rPr>
+              <a:t> DE 1 MILHÃO DE DÓLARES</a:t>
+            </a:r>
+            <a:endParaRPr lang="pt-BR" sz="2000" b="1" i="0">
+              <a:solidFill>
+                <a:srgbClr val="0070C0"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:endParaRPr>
+          </a:p>
+          <a:p>
+            <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR" sz="1300" b="0" i="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:endParaRPr>
+          </a:p>
+          <a:p>
+            <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1300" b="0" i="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1"/>
+                </a:solidFill>
+                <a:effectLst/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:rPr>
+              <a:t>Existe um                                  bem bacana </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1300" b="1" i="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1"/>
+                </a:solidFill>
+                <a:effectLst/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:rPr>
+              <a:t>e muito barato</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1300" b="0" i="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1"/>
+                </a:solidFill>
+                <a:effectLst/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:rPr>
+              <a:t> que é ministrado totalmente online (você faz em casa e na hora que for melhor pra você). Ele possui </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1300" b="1" i="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1"/>
+                </a:solidFill>
+                <a:effectLst/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:rPr>
+              <a:t>6 Módulos</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1300" b="0" i="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1"/>
+                </a:solidFill>
+                <a:effectLst/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:rPr>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1300" b="0" i="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1"/>
+                </a:solidFill>
+                <a:effectLst/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:rPr>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1300" b="0" i="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1"/>
+                </a:solidFill>
+                <a:effectLst/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:rPr>
+              <a:t>distribuídos em diversas vídeo aulas. </a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR" sz="1300" b="0" i="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:endParaRPr>
+          </a:p>
+          <a:p>
+            <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1300" b="0" i="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1"/>
+                </a:solidFill>
+                <a:effectLst/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:rPr>
+              <a:t>Acessando o   </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1300" b="1" i="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1"/>
+                </a:solidFill>
+                <a:effectLst/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:rPr>
+              <a:t>              </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1300" b="1" i="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1"/>
+                </a:solidFill>
+                <a:effectLst/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:rPr>
+              <a:t>Você poderá baixar todas as planilhas grátis do site</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1300" b="0" i="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1"/>
+                </a:solidFill>
+                <a:effectLst/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:rPr>
+              <a:t>. São mais de </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1300" b="1" i="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1"/>
+                </a:solidFill>
+                <a:effectLst/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:rPr>
+              <a:t>40 planilhas prontas.</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1300" b="0" i="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1"/>
+                </a:solidFill>
+                <a:effectLst/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:rPr>
+              <a:t> </a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR" sz="1300" b="0" i="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:endParaRPr>
+          </a:p>
+          <a:p>
+            <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1300" b="1" i="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1"/>
+                </a:solidFill>
+                <a:effectLst/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:rPr>
+              <a:t>                           </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1300" b="0" i="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1"/>
+                </a:solidFill>
+                <a:effectLst/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:rPr>
+              <a:t>você aprende a usar as principais ferramentas do Excel, como formatar células, montar fórmulas, elaborar gráficos e entre outras coisas que você pode  </a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR" sz="1300" b="0" i="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:endParaRPr>
+          </a:p>
+          <a:p>
+            <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1300" b="0" i="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1"/>
+                </a:solidFill>
+                <a:effectLst/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:rPr>
+              <a:t>Ah e não existe mensalidade ta? Você paga o valor do curso e pronto, pode começar a estudar na hora! Para conhecer mais é só </a:t>
+            </a:r>
+            <a:endParaRPr lang="pt-BR" sz="1300">
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+            </a:endParaRPr>
+          </a:p>
+          <a:p>
+            <a:endParaRPr lang="pt-BR" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="6" name="CaixaDeTexto 5">
+            <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2454A64C-CD0D-4EF6-A11A-63D6458A0215}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="7496174" y="904875"/>
+            <a:ext cx="1247775" cy="228600"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="lt1"/>
+          </a:solidFill>
+          <a:ln w="9525" cmpd="sng">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1300" b="1">
+                <a:solidFill>
+                  <a:srgbClr val="0000FF"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t> Curso</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1300" b="1" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="0000FF"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t> de Excel</a:t>
+            </a:r>
+            <a:endParaRPr lang="pt-BR" sz="1300" b="1">
+              <a:solidFill>
+                <a:srgbClr val="0000FF"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="7" name="CaixaDeTexto 6">
+            <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8993E0F9-368C-468C-8A53-17E9F2091054}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="7715250" y="1704975"/>
+            <a:ext cx="600075" cy="228600"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr">
+            <a:noAutofit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1300" b="1">
+                <a:solidFill>
+                  <a:srgbClr val="0000FF"/>
+                </a:solidFill>
+                <a:effectLst/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:rPr>
+              <a:t>Curso</a:t>
+            </a:r>
+            <a:endParaRPr lang="pt-BR" sz="1300">
+              <a:solidFill>
+                <a:srgbClr val="0000FF"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="8" name="CaixaDeTexto 7">
+            <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0B0E4812-AE24-4CDC-A2CB-EBB8EDF65E09}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="6762750" y="2324100"/>
+            <a:ext cx="1057276" cy="209550"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="lt1"/>
+          </a:solidFill>
+          <a:ln w="9525" cmpd="sng">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1300" b="1">
+                <a:solidFill>
+                  <a:srgbClr val="0000FF"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t> Nesse Curso</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="9" name="CaixaDeTexto 8">
+            <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9DAC2B2F-D7D4-438E-939D-07D292334C91}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="10344149" y="3343275"/>
+            <a:ext cx="1885951" cy="180974"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="lt1"/>
+          </a:solidFill>
+          <a:ln w="9525" cmpd="sng">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1300" b="1">
+                <a:solidFill>
+                  <a:srgbClr val="0000FF"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t> clicar aqui e aproveitar!</a:t>
             </a:r>
           </a:p>
         </xdr:txBody>
@@ -1062,10 +1722,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Plan1"/>
-  <dimension ref="A1:H101"/>
+  <dimension ref="A1:Q101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R9" sqref="R9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
@@ -1078,10 +1738,12 @@
     <col min="6" max="6" width="14.5703125" style="6" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="5.28515625" style="7" customWidth="1"/>
     <col min="8" max="8" width="13.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="6"/>
+    <col min="9" max="11" width="9.140625" style="6"/>
+    <col min="12" max="12" width="12.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" s="1" customFormat="1" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>131</v>
       </c>
@@ -1107,7 +1769,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1132,8 +1794,15 @@
       <c r="H2" s="4" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K2" s="12"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="11"/>
+      <c r="N2" s="11"/>
+      <c r="O2" s="11"/>
+      <c r="P2" s="11"/>
+      <c r="Q2" s="11"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <v>2</v>
       </c>
@@ -1158,8 +1827,15 @@
       <c r="H3" s="6" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="11"/>
+      <c r="P3" s="11"/>
+      <c r="Q3" s="11"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1184,8 +1860,15 @@
       <c r="H4" s="4" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="11"/>
+      <c r="N4" s="11"/>
+      <c r="O4" s="11"/>
+      <c r="P4" s="11"/>
+      <c r="Q4" s="11"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>4</v>
       </c>
@@ -1210,8 +1893,15 @@
       <c r="H5" s="6" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="11"/>
+      <c r="N5" s="11"/>
+      <c r="O5" s="11"/>
+      <c r="P5" s="11"/>
+      <c r="Q5" s="11"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1236,8 +1926,15 @@
       <c r="H6" s="4" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="11"/>
+      <c r="O6" s="11"/>
+      <c r="P6" s="11"/>
+      <c r="Q6" s="11"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>6</v>
       </c>
@@ -1262,8 +1959,15 @@
       <c r="H7" s="6" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="11"/>
+      <c r="N7" s="11"/>
+      <c r="O7" s="11"/>
+      <c r="P7" s="11"/>
+      <c r="Q7" s="11"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1288,8 +1992,15 @@
       <c r="H8" s="4" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="11"/>
+      <c r="N8" s="11"/>
+      <c r="O8" s="11"/>
+      <c r="P8" s="11"/>
+      <c r="Q8" s="11"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>8</v>
       </c>
@@ -1314,8 +2025,15 @@
       <c r="H9" s="6" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="11"/>
+      <c r="N9" s="11"/>
+      <c r="O9" s="11"/>
+      <c r="P9" s="11"/>
+      <c r="Q9" s="11"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -1340,8 +2058,15 @@
       <c r="H10" s="4" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
+      <c r="M10" s="11"/>
+      <c r="N10" s="11"/>
+      <c r="O10" s="11"/>
+      <c r="P10" s="11"/>
+      <c r="Q10" s="11"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>10</v>
       </c>
@@ -1366,8 +2091,15 @@
       <c r="H11" s="6" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="11"/>
+      <c r="N11" s="11"/>
+      <c r="O11" s="11"/>
+      <c r="P11" s="11"/>
+      <c r="Q11" s="11"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -1392,8 +2124,15 @@
       <c r="H12" s="4" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K12" s="11"/>
+      <c r="L12" s="11"/>
+      <c r="M12" s="11"/>
+      <c r="N12" s="11"/>
+      <c r="O12" s="11"/>
+      <c r="P12" s="11"/>
+      <c r="Q12" s="11"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
         <v>12</v>
       </c>
@@ -1418,8 +2157,15 @@
       <c r="H13" s="6" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K13" s="11"/>
+      <c r="L13" s="11"/>
+      <c r="M13" s="11"/>
+      <c r="N13" s="11"/>
+      <c r="O13" s="11"/>
+      <c r="P13" s="11"/>
+      <c r="Q13" s="11"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -1444,8 +2190,15 @@
       <c r="H14" s="4" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K14" s="11"/>
+      <c r="L14" s="11"/>
+      <c r="M14" s="11"/>
+      <c r="N14" s="11"/>
+      <c r="O14" s="11"/>
+      <c r="P14" s="11"/>
+      <c r="Q14" s="11"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
         <v>14</v>
       </c>
@@ -1470,8 +2223,15 @@
       <c r="H15" s="6" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K15" s="11"/>
+      <c r="L15" s="11"/>
+      <c r="M15" s="11"/>
+      <c r="N15" s="11"/>
+      <c r="O15" s="11"/>
+      <c r="P15" s="11"/>
+      <c r="Q15" s="11"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -1496,8 +2256,15 @@
       <c r="H16" s="4" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K16" s="11"/>
+      <c r="L16" s="11"/>
+      <c r="M16" s="11"/>
+      <c r="N16" s="11"/>
+      <c r="O16" s="11"/>
+      <c r="P16" s="11"/>
+      <c r="Q16" s="11"/>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
         <v>16</v>
       </c>
@@ -1522,8 +2289,15 @@
       <c r="H17" s="6" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K17" s="11"/>
+      <c r="L17" s="11"/>
+      <c r="M17" s="11"/>
+      <c r="N17" s="11"/>
+      <c r="O17" s="11"/>
+      <c r="P17" s="11"/>
+      <c r="Q17" s="11"/>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -1549,7 +2323,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="7">
         <v>18</v>
       </c>
@@ -1575,7 +2349,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -1601,7 +2375,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="7">
         <v>20</v>
       </c>
@@ -1627,7 +2401,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -1653,7 +2427,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="7">
         <v>22</v>
       </c>
@@ -1679,7 +2453,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -1705,7 +2479,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="7">
         <v>24</v>
       </c>
@@ -1731,7 +2505,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -1757,7 +2531,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="7">
         <v>26</v>
       </c>
@@ -1783,7 +2557,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -1809,7 +2583,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="7">
         <v>28</v>
       </c>
@@ -1835,7 +2609,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -1861,7 +2635,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="7">
         <v>30</v>
       </c>
@@ -1887,7 +2661,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>31</v>
       </c>

</xml_diff>